<commit_message>
añadidas horas semana 3
</commit_message>
<xml_diff>
--- a/Conocimiento/Metodología/Calculadora (version 1).xlsx
+++ b/Conocimiento/Metodología/Calculadora (version 1).xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesos\Desktop\ISPP proyecto\ISPP_A4MJ\Conocimiento\Metodología\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="7152" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7155" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Costes y presupuesto" sheetId="2" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="Imputaciones semana" sheetId="3" r:id="rId4"/>
     <sheet name="Hoja2" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -23,7 +28,7 @@
     <author>Ale Garrido Resina</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0">
+    <comment ref="E4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0">
+    <comment ref="E6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0">
+    <comment ref="D7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -157,7 +162,7 @@
     <author>Ale Garrido Resina</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -414,7 +419,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -1339,10 +1344,11 @@
     <cellStyle name="60% - Énfasis4" xfId="34" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="38" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="42" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="7" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="12" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="14" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="3" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="6" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="19" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="23" builtinId="33" customBuiltin="1"/>
@@ -1361,7 +1367,6 @@
     <cellStyle name="Texto de advertencia" xfId="15" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="17" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título" xfId="2" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="3" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="4" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="5" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
@@ -1380,7 +1385,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1417,9 +1422,12 @@
             <c:strRef>
               <c:f>Caculadora!$G$1:$G$2</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Progreso Real</c:v>
+                  <c:v>Progreso</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1491,7 +1499,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-E409-4349-BB70-B4830E9B9444}"/>
@@ -1533,7 +1541,8 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
@@ -1542,8 +1551,8 @@
                     <a:ln w="9525">
                       <a:solidFill>
                         <a:schemeClr val="lt1">
-                          <a:lumMod val="95%"/>
-                          <a:alpha val="54%"/>
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
                         </a:schemeClr>
                       </a:solidFill>
                     </a:ln>
@@ -1560,23 +1569,12 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.16164377259962187</c:v>
+                  <c:v>0.21822715717406069</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:datalabelsRange>
-                <c15:f>Caculadora!$G$5</c15:f>
-                <c15:dlblRangeCache>
-                  <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>4688(16%)</c:v>
-                  </c:pt>
-                </c15:dlblRangeCache>
-              </c15:datalabelsRange>
-            </c:ext>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E409-4349-BB70-B4830E9B9444}"/>
             </c:ext>
@@ -1589,9 +1587,12 @@
             <c:strRef>
               <c:f>Caculadora!$H$1:$H$2</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Progreso Objetivo</c:v>
+                  <c:v>Progreso</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Objetivo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1624,7 +1625,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4706F960-E611-4E7F-B0C2-57CB3561C6F1}" type="CELLRANGE">
+                    <a:fld id="{934BDDEB-C00D-4F62-BB7D-E557FB84EF1D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1639,7 +1640,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1681,7 +1682,8 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
@@ -1690,8 +1692,8 @@
                     <a:ln w="9525">
                       <a:solidFill>
                         <a:schemeClr val="lt1">
-                          <a:lumMod val="95%"/>
-                          <a:alpha val="54%"/>
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
                         </a:schemeClr>
                       </a:solidFill>
                     </a:ln>
@@ -1713,7 +1715,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
                 <c15:f>Caculadora!$H$4</c15:f>
@@ -1766,7 +1768,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="b" anchorCtr="0"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="b" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1817,14 +1819,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -1852,7 +1854,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1930,7 +1932,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0CCE-482A-8138-6F93BA323EB6}"/>
             </c:ext>
@@ -1938,7 +1940,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Estimado</c:v>
           </c:tx>
@@ -2024,7 +2026,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0CCE-482A-8138-6F93BA323EB6}"/>
             </c:ext>
@@ -2042,7 +2044,7 @@
         <c:smooth val="0"/>
         <c:axId val="322951680"/>
         <c:axId val="320142080"/>
-        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+        <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
@@ -2168,6 +2170,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2265,17 +2287,7 @@
               </a:p>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
+                  <a:defRPr/>
                 </a:pPr>
                 <a:endParaRPr lang="es-ES"/>
               </a:p>
@@ -2289,6 +2301,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="#,##0.00\ &quot;€&quot;" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2376,14 +2408,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2419,7 +2451,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2497,7 +2529,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5661-4738-B608-7F29A7F5D55D}"/>
             </c:ext>
@@ -2505,7 +2537,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Estimado</c:v>
           </c:tx>
@@ -2591,7 +2623,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5661-4738-B608-7F29A7F5D55D}"/>
             </c:ext>
@@ -2609,7 +2641,7 @@
         <c:smooth val="0"/>
         <c:axId val="324195840"/>
         <c:axId val="324018176"/>
-        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+        <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
@@ -2785,14 +2817,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2828,7 +2860,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2860,7 +2892,7 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Hoja1!$H$1</c:f>
@@ -2911,7 +2943,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000006-EB81-4B8A-9CC2-7323559F094F}"/>
               </c:ext>
@@ -2926,7 +2958,7 @@
               </c:pt>
             </c:numLit>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-EB81-4B8A-9CC2-7323559F094F}"/>
             </c:ext>
@@ -2934,7 +2966,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Hoja1!$G$1</c:f>
@@ -2994,7 +3026,7 @@
               </c:pt>
             </c:numLit>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-EB81-4B8A-9CC2-7323559F094F}"/>
             </c:ext>
@@ -3012,7 +3044,7 @@
         <c:overlap val="100"/>
         <c:axId val="324196864"/>
         <c:axId val="324019904"/>
-        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+        <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
               <c15:ser>
@@ -3038,25 +3070,25 @@
                 <c:spPr>
                   <a:gradFill rotWithShape="1">
                     <a:gsLst>
-                      <a:gs pos="0%">
+                      <a:gs pos="0">
                         <a:schemeClr val="accent1">
-                          <a:satMod val="103%"/>
-                          <a:lumMod val="102%"/>
-                          <a:tint val="94%"/>
+                          <a:satMod val="103000"/>
+                          <a:lumMod val="102000"/>
+                          <a:tint val="94000"/>
                         </a:schemeClr>
                       </a:gs>
-                      <a:gs pos="50%">
+                      <a:gs pos="50000">
                         <a:schemeClr val="accent1">
-                          <a:satMod val="110%"/>
-                          <a:lumMod val="100%"/>
-                          <a:shade val="100%"/>
+                          <a:satMod val="110000"/>
+                          <a:lumMod val="100000"/>
+                          <a:shade val="100000"/>
                         </a:schemeClr>
                       </a:gs>
-                      <a:gs pos="100%">
+                      <a:gs pos="100000">
                         <a:schemeClr val="accent1">
-                          <a:lumMod val="99%"/>
-                          <a:satMod val="120%"/>
-                          <a:shade val="78%"/>
+                          <a:lumMod val="99000"/>
+                          <a:satMod val="120000"/>
+                          <a:shade val="78000"/>
                         </a:schemeClr>
                       </a:gs>
                     </a:gsLst>
@@ -3068,7 +3100,7 @@
                   <a:effectLst>
                     <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
                       <a:srgbClr val="000000">
-                        <a:alpha val="63%"/>
+                        <a:alpha val="63000"/>
                       </a:srgbClr>
                     </a:outerShdw>
                   </a:effectLst>
@@ -3167,14 +3199,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -3202,7 +3234,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -3239,6 +3271,11 @@
             <c:spPr>
               <a:ln w="44450"/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-38B4-46DF-BC24-A92988660D8E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -3286,6 +3323,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-38B4-46DF-BC24-A92988660D8E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3345,6 +3387,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-38B4-46DF-BC24-A92988660D8E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3354,7 +3401,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="323339776"/>
         <c:axId val="324023360"/>
@@ -3384,7 +3430,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
@@ -3431,7 +3476,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3455,7 +3499,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3511,7 +3554,7 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
@@ -3520,38 +3563,38 @@
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
-    <a:lumMod val="60%"/>
+    <a:lumMod val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80%"/>
-    <a:lumOff val="20%"/>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80%"/>
+    <a:lumMod val="80000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60%"/>
-    <a:lumOff val="40%"/>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50%"/>
+    <a:lumMod val="50000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70%"/>
-    <a:lumOff val="30%"/>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70%"/>
+    <a:lumMod val="70000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50%"/>
-    <a:lumOff val="50%"/>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
@@ -3560,38 +3603,38 @@
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
-    <a:lumMod val="60%"/>
+    <a:lumMod val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80%"/>
-    <a:lumOff val="20%"/>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80%"/>
+    <a:lumMod val="80000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60%"/>
-    <a:lumOff val="40%"/>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50%"/>
+    <a:lumMod val="50000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70%"/>
-    <a:lumOff val="30%"/>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70%"/>
+    <a:lumMod val="70000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50%"/>
-    <a:lumOff val="50%"/>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
@@ -3600,38 +3643,38 @@
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
-    <a:lumMod val="60%"/>
+    <a:lumMod val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80%"/>
-    <a:lumOff val="20%"/>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80%"/>
+    <a:lumMod val="80000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60%"/>
-    <a:lumOff val="40%"/>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50%"/>
+    <a:lumMod val="50000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70%"/>
-    <a:lumOff val="30%"/>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70%"/>
+    <a:lumMod val="70000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50%"/>
-    <a:lumOff val="50%"/>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
@@ -3640,45 +3683,45 @@
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
-    <a:lumMod val="60%"/>
+    <a:lumMod val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80%"/>
-    <a:lumOff val="20%"/>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80%"/>
+    <a:lumMod val="80000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60%"/>
-    <a:lumOff val="40%"/>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50%"/>
+    <a:lumMod val="50000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70%"/>
-    <a:lumOff val="30%"/>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70%"/>
+    <a:lumMod val="70000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50%"/>
-    <a:lumOff val="50%"/>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" id="328">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="328">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
@@ -3689,15 +3732,15 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="54%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3715,21 +3758,21 @@
     <cs:spPr>
       <a:gradFill flip="none" rotWithShape="1">
         <a:gsLst>
-          <a:gs pos="0%">
+          <a:gs pos="0">
             <a:schemeClr val="dk1">
-              <a:lumMod val="65%"/>
-              <a:lumOff val="35%"/>
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
             </a:schemeClr>
           </a:gs>
-          <a:gs pos="100%">
+          <a:gs pos="100000">
             <a:schemeClr val="dk1">
-              <a:lumMod val="85%"/>
-              <a:lumOff val="15%"/>
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
             </a:schemeClr>
           </a:gs>
         </a:gsLst>
         <a:path path="circle">
-          <a:fillToRect l="50%" t="50%" r="50%" b="50%"/>
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
         </a:path>
         <a:tileRect/>
       </a:gradFill>
@@ -3742,7 +3785,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3753,8 +3796,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -3850,15 +3893,15 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="54%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3875,28 +3918,28 @@
     <cs:spPr>
       <a:gradFill>
         <a:gsLst>
-          <a:gs pos="100%">
+          <a:gs pos="100000">
             <a:schemeClr val="dk1">
-              <a:lumMod val="95%"/>
-              <a:lumOff val="5%"/>
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
             </a:schemeClr>
           </a:gs>
-          <a:gs pos="0%">
+          <a:gs pos="0">
             <a:schemeClr val="dk1">
-              <a:lumMod val="75%"/>
-              <a:lumOff val="25%"/>
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
             </a:schemeClr>
           </a:gs>
         </a:gsLst>
         <a:path path="circle">
-          <a:fillToRect l="50%" t="50%" r="50%" b="50%"/>
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
         </a:path>
       </a:gradFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="75%"/>
-            <a:lumOff val="25%"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3929,7 +3972,7 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3955,8 +3998,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="10%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3974,8 +4017,8 @@
       <a:ln>
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="5%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4008,8 +4051,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="54%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4021,7 +4064,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4048,15 +4091,15 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="54%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4075,8 +4118,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="54%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4089,14 +4132,14 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="95%"/>
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0%">
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
       <a:effectLst>
         <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
           <a:prstClr val="black">
-            <a:alpha val="40%"/>
+            <a:alpha val="40000"/>
           </a:prstClr>
         </a:outerShdw>
       </a:effectLst>
@@ -4125,7 +4168,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4140,17 +4183,17 @@
     <cs:spPr>
       <a:gradFill>
         <a:gsLst>
-          <a:gs pos="100%">
+          <a:gs pos="100000">
             <a:schemeClr val="lt1">
-              <a:lumMod val="85%"/>
+              <a:lumMod val="85000"/>
             </a:schemeClr>
           </a:gs>
-          <a:gs pos="0%">
+          <a:gs pos="0">
             <a:schemeClr val="lt1"/>
           </a:gs>
         </a:gsLst>
         <a:path path="circle">
-          <a:fillToRect l="50%" t="50%" r="50%" b="50%"/>
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
         </a:path>
       </a:gradFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -4167,7 +4210,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4184,15 +4227,15 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="1000" kern="1200"/>
@@ -4203,16 +4246,16 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15%"/>
-            <a:lumOff val="85%"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4234,8 +4277,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15%"/>
-            <a:lumOff val="85%"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4249,8 +4292,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75%"/>
-        <a:lumOff val="25%"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4261,8 +4304,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -4272,8 +4315,8 @@
       <a:ln>
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="25%"/>
-            <a:lumOff val="75%"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4365,8 +4408,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -4374,8 +4417,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15%"/>
-            <a:lumOff val="85%"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4393,15 +4436,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65%"/>
-          <a:lumOff val="35%"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65%"/>
-            <a:lumOff val="35%"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4418,8 +4461,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="35%"/>
-            <a:lumOff val="65%"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4437,8 +4480,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65%"/>
-            <a:lumOff val="35%"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4470,8 +4513,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15%"/>
-            <a:lumOff val="85%"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4489,8 +4532,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="5%"/>
-            <a:lumOff val="95%"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4508,8 +4551,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75%"/>
-            <a:lumOff val="25%"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4527,8 +4570,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="35%"/>
-            <a:lumOff val="65%"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4541,8 +4584,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4569,8 +4612,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4586,8 +4629,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="35%"/>
-            <a:lumOff val="65%"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4600,11 +4643,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0%"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4630,8 +4673,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4650,8 +4693,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15%"/>
-            <a:lumOff val="85%"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4663,8 +4706,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4687,15 +4730,15 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="1000" kern="1200"/>
@@ -4706,16 +4749,16 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15%"/>
-            <a:lumOff val="85%"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4737,8 +4780,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15%"/>
-            <a:lumOff val="85%"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4752,8 +4795,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75%"/>
-        <a:lumOff val="25%"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4764,8 +4807,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -4775,8 +4818,8 @@
       <a:ln>
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="25%"/>
-            <a:lumOff val="75%"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4868,8 +4911,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -4877,8 +4920,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15%"/>
-            <a:lumOff val="85%"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4896,15 +4939,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65%"/>
-          <a:lumOff val="35%"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65%"/>
-            <a:lumOff val="35%"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4921,8 +4964,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="35%"/>
-            <a:lumOff val="65%"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4940,8 +4983,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65%"/>
-            <a:lumOff val="35%"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4973,8 +5016,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15%"/>
-            <a:lumOff val="85%"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4992,8 +5035,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="5%"/>
-            <a:lumOff val="95%"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5011,8 +5054,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75%"/>
-            <a:lumOff val="25%"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5030,8 +5073,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="35%"/>
-            <a:lumOff val="65%"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5044,8 +5087,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5072,8 +5115,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5089,8 +5132,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="35%"/>
-            <a:lumOff val="65%"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5103,11 +5146,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0%"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -5133,8 +5176,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5153,8 +5196,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15%"/>
-            <a:lumOff val="85%"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -5166,8 +5209,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5190,14 +5233,14 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" id="328">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="328">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
@@ -5208,15 +5251,15 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="54%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5234,21 +5277,21 @@
     <cs:spPr>
       <a:gradFill flip="none" rotWithShape="1">
         <a:gsLst>
-          <a:gs pos="0%">
+          <a:gs pos="0">
             <a:schemeClr val="dk1">
-              <a:lumMod val="65%"/>
-              <a:lumOff val="35%"/>
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
             </a:schemeClr>
           </a:gs>
-          <a:gs pos="100%">
+          <a:gs pos="100000">
             <a:schemeClr val="dk1">
-              <a:lumMod val="85%"/>
-              <a:lumOff val="15%"/>
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
             </a:schemeClr>
           </a:gs>
         </a:gsLst>
         <a:path path="circle">
-          <a:fillToRect l="50%" t="50%" r="50%" b="50%"/>
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
         </a:path>
         <a:tileRect/>
       </a:gradFill>
@@ -5261,7 +5304,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5272,8 +5315,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="65%"/>
-        <a:lumOff val="35%"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -5369,15 +5412,15 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="54%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -5394,28 +5437,28 @@
     <cs:spPr>
       <a:gradFill>
         <a:gsLst>
-          <a:gs pos="100%">
+          <a:gs pos="100000">
             <a:schemeClr val="dk1">
-              <a:lumMod val="95%"/>
-              <a:lumOff val="5%"/>
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
             </a:schemeClr>
           </a:gs>
-          <a:gs pos="0%">
+          <a:gs pos="0">
             <a:schemeClr val="dk1">
-              <a:lumMod val="75%"/>
-              <a:lumOff val="25%"/>
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
             </a:schemeClr>
           </a:gs>
         </a:gsLst>
         <a:path path="circle">
-          <a:fillToRect l="50%" t="50%" r="50%" b="50%"/>
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
         </a:path>
       </a:gradFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="75%"/>
-            <a:lumOff val="25%"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -5448,7 +5491,7 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5474,8 +5517,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="10%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5493,8 +5536,8 @@
       <a:ln>
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="5%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -5527,8 +5570,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="54%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -5540,7 +5583,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5567,15 +5610,15 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="54%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5594,8 +5637,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
-            <a:lumMod val="95%"/>
-            <a:alpha val="54%"/>
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5608,14 +5651,14 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="95%"/>
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0%">
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
       <a:effectLst>
         <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
           <a:prstClr val="black">
-            <a:alpha val="40%"/>
+            <a:alpha val="40000"/>
           </a:prstClr>
         </a:outerShdw>
       </a:effectLst>
@@ -5644,7 +5687,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5659,17 +5702,17 @@
     <cs:spPr>
       <a:gradFill>
         <a:gsLst>
-          <a:gs pos="100%">
+          <a:gs pos="100000">
             <a:schemeClr val="lt1">
-              <a:lumMod val="85%"/>
+              <a:lumMod val="85000"/>
             </a:schemeClr>
           </a:gs>
-          <a:gs pos="0%">
+          <a:gs pos="0">
             <a:schemeClr val="lt1"/>
           </a:gs>
         </a:gsLst>
         <a:path path="circle">
-          <a:fillToRect l="50%" t="50%" r="50%" b="50%"/>
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
         </a:path>
       </a:gradFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -5686,7 +5729,7 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1">
-        <a:lumMod val="85%"/>
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -5722,7 +5765,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4478CC80-9EF6-4ADD-B060-B7DA1112C280}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4478CC80-9EF6-4ADD-B060-B7DA1112C280}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5760,7 +5803,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46D435CB-CF32-4D44-8F73-691DA66C623B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46D435CB-CF32-4D44-8F73-691DA66C623B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5803,7 +5846,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15DB4FA1-CE3C-4ABC-8972-8E314AEC1C7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15DB4FA1-CE3C-4ABC-8972-8E314AEC1C7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5841,7 +5884,7 @@
         <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1428A001-ABB8-4817-8FF8-E1823E570921}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1428A001-ABB8-4817-8FF8-E1823E570921}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5878,7 +5921,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="3 CuadroTexto"/>
+            <xdr:cNvPr id="4" name="3 CuadroTexto">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -6012,7 +6061,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="4 CuadroTexto"/>
+            <xdr:cNvPr id="5" name="4 CuadroTexto">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -6149,7 +6204,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="8 Gráfico"/>
+        <xdr:cNvPr id="9" name="8 Gráfico">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6456,7 +6517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6466,21 +6527,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -6506,7 +6567,7 @@
       <c r="L1" s="83"/>
       <c r="M1" s="84"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>8</v>
       </c>
@@ -6540,7 +6601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="19"/>
       <c r="C3" s="52" t="s">
@@ -6571,7 +6632,7 @@
         <v>466.66666666666669</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="53" t="s">
@@ -6593,7 +6654,7 @@
         <v>16088</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>9</v>
       </c>
@@ -6612,7 +6673,7 @@
         <v>466.66666666666669</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="19"/>
       <c r="C6" s="55" t="s">
@@ -6629,7 +6690,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="C7" s="56" t="s">
@@ -6650,7 +6711,7 @@
         <v>4748.666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>16</v>
       </c>
@@ -6659,7 +6720,7 @@
         <v>20754.666666666668</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>14</v>
       </c>
@@ -6674,7 +6735,7 @@
         <v>4150.9333333333334</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>15</v>
       </c>
@@ -6689,7 +6750,7 @@
         <v>4150.9333333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E11" s="16" t="s">
         <v>10</v>
       </c>
@@ -6698,7 +6759,7 @@
         <v>29056.533333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -6706,7 +6767,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -6730,11 +6791,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G1:H1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G1">
@@ -6755,19 +6816,19 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="85" t="s">
         <v>19</v>
       </c>
@@ -6784,7 +6845,7 @@
       </c>
       <c r="K1" s="90"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
         <v>1</v>
       </c>
@@ -6813,13 +6874,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="65">
         <f>SUM('Imputaciones semana'!A$2:A$30)</f>
-        <v>33.1</v>
+        <v>49.1</v>
       </c>
       <c r="C3" s="66">
         <v>27.19</v>
@@ -6830,11 +6891,11 @@
       </c>
       <c r="E3" s="68">
         <f t="shared" ref="E3:E9" si="0">B3*C3</f>
-        <v>899.98900000000003</v>
+        <v>1335.029</v>
       </c>
       <c r="G3" s="62">
         <f>(E10+K3)/L13</f>
-        <v>0.16164377259962187</v>
+        <v>0.21822715717406069</v>
       </c>
       <c r="H3" s="62">
         <v>1</v>
@@ -6847,40 +6908,40 @@
         <v>1537.1666666666667</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="69">
         <f>SUM('Imputaciones semana'!B$2:B$30)</f>
-        <v>29</v>
+        <v>49.75</v>
       </c>
       <c r="C4" s="70">
         <v>11.47</v>
       </c>
       <c r="D4" s="71">
         <f t="shared" ref="D4:D9" si="1">HOUR(B4)+MINUTE(B4)/60+SECOND(B4)/3600</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E4" s="72">
         <f t="shared" si="0"/>
-        <v>332.63</v>
+        <v>570.63250000000005</v>
       </c>
       <c r="G4" s="63">
         <f>G3*H4</f>
-        <v>4687.6694053890342</v>
+        <v>6328.5875580477596</v>
       </c>
       <c r="H4" s="64">
         <v>29000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="69">
         <f>SUM('Imputaciones semana'!C$2:C$30)</f>
-        <v>34.6</v>
+        <v>49.6</v>
       </c>
       <c r="C5" s="70">
         <v>11.47</v>
@@ -6891,39 +6952,39 @@
       </c>
       <c r="E5" s="72">
         <f t="shared" si="0"/>
-        <v>396.86200000000002</v>
+        <v>568.91200000000003</v>
       </c>
       <c r="G5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="69">
         <f>SUM('Imputaciones semana'!D$2:D$30)</f>
-        <v>24.5</v>
+        <v>36.25</v>
       </c>
       <c r="C6" s="70">
         <v>11.47</v>
       </c>
       <c r="D6" s="71">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E6" s="72">
         <f t="shared" si="0"/>
-        <v>281.01500000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>415.78750000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="69">
         <f>SUM('Imputaciones semana'!E$2:E$30)</f>
-        <v>46.5</v>
+        <v>67.5</v>
       </c>
       <c r="C7" s="70">
         <v>16.010000000000002</v>
@@ -6934,63 +6995,63 @@
       </c>
       <c r="E7" s="72">
         <f t="shared" si="0"/>
-        <v>744.46500000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1080.6750000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="69">
         <f>SUM('Imputaciones semana'!F$2:F$30)</f>
-        <v>17</v>
+        <v>30.5</v>
       </c>
       <c r="C8" s="70">
         <v>11.47</v>
       </c>
       <c r="D8" s="71">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E8" s="72">
         <f t="shared" si="0"/>
-        <v>194.99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>349.83500000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="78" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="73">
         <f>SUM('Imputaciones semana'!G$2:G$30)</f>
-        <v>27</v>
+        <v>42.1</v>
       </c>
       <c r="C9" s="74">
         <v>11.47</v>
       </c>
       <c r="D9" s="75">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="E9" s="76">
         <f t="shared" si="0"/>
-        <v>309.69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>482.88700000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>211.7</v>
+        <v>324.8</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="4">
         <f>SUM(E3:E9)</f>
-        <v>3159.6410000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>4803.7580000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="86" t="s">
         <v>20</v>
       </c>
@@ -7002,7 +7063,7 @@
       <c r="G12" s="86"/>
       <c r="H12" s="86"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>29</v>
       </c>
@@ -7035,7 +7096,7 @@
         <v>29056.533333333336</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -7083,7 +7144,7 @@
         <v>1816.0333333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
@@ -7131,7 +7192,7 @@
         <v>3632.0666666666671</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>23</v>
       </c>
@@ -7179,45 +7240,45 @@
         <v>5448.1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="36">
         <f>('Imputaciones semana'!A5)*$C$3</f>
-        <v>0</v>
+        <v>435.04</v>
       </c>
       <c r="C17" s="37">
         <f>('Imputaciones semana'!B5)*$C$4</f>
-        <v>0</v>
+        <v>238.00250000000003</v>
       </c>
       <c r="D17" s="37">
         <f>('Imputaciones semana'!C5)*$C$5</f>
-        <v>0</v>
+        <v>172.05</v>
       </c>
       <c r="E17" s="37">
         <f>('Imputaciones semana'!D5)*$C$6</f>
-        <v>0</v>
+        <v>134.77250000000001</v>
       </c>
       <c r="F17" s="37">
         <f>('Imputaciones semana'!E5)*$C$7</f>
-        <v>0</v>
+        <v>336.21000000000004</v>
       </c>
       <c r="G17" s="37">
         <f>('Imputaciones semana'!F5)*$C$8</f>
-        <v>0</v>
+        <v>154.845</v>
       </c>
       <c r="H17" s="38">
         <f>('Imputaciones semana'!G5)*$C$9</f>
-        <v>0</v>
+        <v>173.197</v>
       </c>
       <c r="I17" s="43">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1644.1170000000002</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K17">
         <v>4</v>
@@ -7227,7 +7288,7 @@
         <v>7264.1333333333341</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -7265,7 +7326,7 @@
       </c>
       <c r="J18" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K18">
         <v>5</v>
@@ -7275,7 +7336,7 @@
         <v>9080.1666666666679</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
@@ -7313,7 +7374,7 @@
       </c>
       <c r="J19" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K19">
         <v>6</v>
@@ -7323,7 +7384,7 @@
         <v>10896.2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>27</v>
       </c>
@@ -7361,7 +7422,7 @@
       </c>
       <c r="J20" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K20">
         <v>7</v>
@@ -7371,7 +7432,7 @@
         <v>12712.233333333335</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="36">
         <f>('Imputaciones semana'!A9)*$C$3</f>
         <v>0</v>
@@ -7406,7 +7467,7 @@
       </c>
       <c r="J21" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K21">
         <v>8</v>
@@ -7416,7 +7477,7 @@
         <v>14528.266666666668</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="39">
         <f>('Imputaciones semana'!A10)*$C$3</f>
         <v>0</v>
@@ -7451,7 +7512,7 @@
       </c>
       <c r="J22" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K22">
         <v>9</v>
@@ -7461,7 +7522,7 @@
         <v>16344.300000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="36">
         <f>('Imputaciones semana'!A11)*$C$3</f>
         <v>0</v>
@@ -7496,7 +7557,7 @@
       </c>
       <c r="J23" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K23">
         <v>10</v>
@@ -7506,7 +7567,7 @@
         <v>18160.333333333336</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="39">
         <f>('Imputaciones semana'!A12)*$C$3</f>
         <v>0</v>
@@ -7541,7 +7602,7 @@
       </c>
       <c r="J24" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K24">
         <v>11</v>
@@ -7551,7 +7612,7 @@
         <v>19976.366666666669</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" s="36">
         <f>('Imputaciones semana'!A13)*$C$3</f>
         <v>0</v>
@@ -7586,7 +7647,7 @@
       </c>
       <c r="J25" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K25">
         <v>12</v>
@@ -7596,7 +7657,7 @@
         <v>21792.400000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="39">
         <f>('Imputaciones semana'!A14)*$C$3</f>
         <v>0</v>
@@ -7631,7 +7692,7 @@
       </c>
       <c r="J26" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K26">
         <v>13</v>
@@ -7641,7 +7702,7 @@
         <v>23608.433333333334</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="36">
         <f>('Imputaciones semana'!A15)*$C$3</f>
         <v>0</v>
@@ -7676,7 +7737,7 @@
       </c>
       <c r="J27" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K27">
         <v>14</v>
@@ -7686,7 +7747,7 @@
         <v>25424.466666666671</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="39">
         <f>('Imputaciones semana'!A16)*$C$3</f>
         <v>0</v>
@@ -7721,7 +7782,7 @@
       </c>
       <c r="J28" s="4">
         <f t="shared" si="3"/>
-        <v>3159.641000000001</v>
+        <v>4803.7580000000016</v>
       </c>
       <c r="K28">
         <v>15</v>
@@ -7731,7 +7792,7 @@
         <v>27240.500000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K29">
         <v>16</v>
       </c>
@@ -7740,41 +7801,41 @@
         <v>29056.533333333336</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B30" s="4">
         <f t="shared" ref="B30:H30" si="4">SUM(B14:B20)</f>
-        <v>899.98900000000003</v>
+        <v>1335.029</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="4"/>
-        <v>332.63</v>
+        <v>570.63250000000005</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="4"/>
-        <v>396.86200000000002</v>
+        <v>568.91200000000003</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="4"/>
-        <v>281.01500000000004</v>
+        <v>415.78750000000002</v>
       </c>
       <c r="F30" s="4">
         <f t="shared" si="4"/>
-        <v>744.46500000000003</v>
+        <v>1080.6750000000002</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="4"/>
-        <v>194.99</v>
+        <v>349.83500000000004</v>
       </c>
       <c r="H30" s="4">
         <f t="shared" si="4"/>
-        <v>309.69</v>
+        <v>482.887</v>
       </c>
       <c r="I30" s="4">
         <f>SUM(B30:H30)</f>
-        <v>3159.6410000000001</v>
+        <v>4803.7580000000007</v>
       </c>
     </row>
   </sheetData>
@@ -7794,17 +7855,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" activeCellId="6" sqref="G5 F5 E5 D5 C5 B5 A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -7827,7 +7888,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="35">
         <v>10</v>
       </c>
@@ -7856,7 +7917,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="35">
         <v>17.600000000000001</v>
       </c>
@@ -7885,7 +7946,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="35">
         <v>5.5</v>
       </c>
@@ -7914,19 +7975,33 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="35">
+        <v>16</v>
+      </c>
+      <c r="B5" s="35">
+        <v>20.75</v>
+      </c>
+      <c r="C5" s="35">
+        <v>15</v>
+      </c>
+      <c r="D5" s="35">
+        <v>11.75</v>
+      </c>
+      <c r="E5" s="35">
+        <v>21</v>
+      </c>
+      <c r="F5" s="35">
+        <v>13.5</v>
+      </c>
+      <c r="G5" s="35">
+        <v>15.1</v>
+      </c>
       <c r="H5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -7938,7 +8013,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -7950,7 +8025,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -7962,7 +8037,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -7974,7 +8049,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -7986,7 +8061,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -7998,7 +8073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -8008,7 +8083,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -8018,7 +8093,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -8028,7 +8103,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -8038,7 +8113,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -8048,7 +8123,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -8058,7 +8133,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -8068,7 +8143,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -8078,7 +8153,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -8088,7 +8163,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -8098,7 +8173,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -8108,7 +8183,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -8118,7 +8193,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -8128,7 +8203,7 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -8138,7 +8213,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -8148,7 +8223,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -8158,7 +8233,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -8168,7 +8243,7 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -8178,7 +8253,7 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -8197,13 +8272,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>29000</v>
       </c>
@@ -8223,7 +8298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1/12</f>
         <v>2416.6666666666665</v>
@@ -8246,7 +8321,7 @@
         <v>333.33333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2400</v>
       </c>
@@ -8268,7 +8343,7 @@
         <v>458.33333333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>65</v>
       </c>
@@ -8284,7 +8359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
         <v>71</v>
       </c>
@@ -8296,7 +8371,7 @@
         <v>416.66666666666669</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
         <v>71</v>
       </c>
@@ -8308,7 +8383,7 @@
         <v>595.83333333333337</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -8329,7 +8404,7 @@
         <v>500.00000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -8352,7 +8427,7 @@
         <v>733.33333333333337</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -8375,7 +8450,7 @@
         <v>58.333333333333336</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -8398,7 +8473,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -8421,7 +8496,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -8444,7 +8519,7 @@
         <v>58.333333333333336</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -8461,7 +8536,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -8478,7 +8553,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
@@ -8491,7 +8566,7 @@
         <v>10333.333333333334</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
@@ -8504,7 +8579,7 @@
         <v>12900</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -8524,7 +8599,7 @@
         <v>791.66666666666674</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -8544,7 +8619,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
@@ -8564,7 +8639,7 @@
         <v>1291.6666666666667</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H20" t="s">
         <v>72</v>
       </c>

</xml_diff>